<commit_message>
Filled in 75% of battery data. Parser script is modified to get values for charging HPPC at the moment
</commit_message>
<xml_diff>
--- a/lapsim/VTC6_Data.xlsx
+++ b/lapsim/VTC6_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Github\LapSim\lapsim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9F3B38-3C25-421E-BBF7-6B63CAC4AB25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0A8507-330A-4984-8BF3-B22F36D0C2AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C80E3676-C200-4ED4-9617-336096DD9BF4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>SOC</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>See PER Docs</t>
+  </si>
+  <si>
+    <t>Correlation %</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
   <dimension ref="A1:T1646"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,7 +437,8 @@
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
     <col min="7" max="7" width="10.21875" customWidth="1"/>
     <col min="8" max="8" width="10.5546875" customWidth="1"/>
-    <col min="12" max="13" width="10.77734375" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" customWidth="1"/>
     <col min="15" max="15" width="10.21875" customWidth="1"/>
     <col min="16" max="16" width="10.33203125" customWidth="1"/>
     <col min="20" max="20" width="10.88671875" customWidth="1"/>
@@ -486,7 +490,7 @@
         <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N3" t="s">
         <v>0</v>
@@ -521,13 +525,34 @@
         <v>100</v>
       </c>
       <c r="G4">
-        <v>1.96</v>
+        <v>1.62</v>
       </c>
       <c r="H4">
         <v>2.4</v>
       </c>
       <c r="I4">
         <v>1996</v>
+      </c>
+      <c r="N4">
+        <v>99.928600000000003</v>
+      </c>
+      <c r="O4">
+        <v>1.72</v>
+      </c>
+      <c r="P4">
+        <v>4.37</v>
+      </c>
+      <c r="Q4">
+        <v>3429</v>
+      </c>
+      <c r="R4">
+        <v>67879</v>
+      </c>
+      <c r="S4">
+        <v>68239</v>
+      </c>
+      <c r="T4">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -552,6 +577,27 @@
       <c r="L5">
         <v>94.6</v>
       </c>
+      <c r="N5">
+        <v>99.167000000000002</v>
+      </c>
+      <c r="O5">
+        <v>1.63</v>
+      </c>
+      <c r="P5">
+        <v>3.27</v>
+      </c>
+      <c r="Q5">
+        <v>3451</v>
+      </c>
+      <c r="R5">
+        <v>67398</v>
+      </c>
+      <c r="S5">
+        <v>67758</v>
+      </c>
+      <c r="T5">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C6">
@@ -581,6 +627,27 @@
       <c r="L6">
         <v>88</v>
       </c>
+      <c r="N6">
+        <v>85.560699999999997</v>
+      </c>
+      <c r="O6">
+        <v>1.54</v>
+      </c>
+      <c r="P6">
+        <v>2.71</v>
+      </c>
+      <c r="Q6">
+        <v>3537</v>
+      </c>
+      <c r="R6">
+        <v>66917</v>
+      </c>
+      <c r="S6">
+        <v>67277</v>
+      </c>
+      <c r="T6">
+        <v>97</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C7">
@@ -610,6 +677,27 @@
       <c r="L7">
         <v>96</v>
       </c>
+      <c r="N7">
+        <v>73.278899999999993</v>
+      </c>
+      <c r="O7">
+        <v>1.54</v>
+      </c>
+      <c r="P7">
+        <v>5.04</v>
+      </c>
+      <c r="Q7">
+        <v>7573</v>
+      </c>
+      <c r="R7">
+        <v>66436</v>
+      </c>
+      <c r="S7">
+        <v>66796</v>
+      </c>
+      <c r="T7">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C8">
@@ -639,6 +727,27 @@
       <c r="L8">
         <v>96</v>
       </c>
+      <c r="N8">
+        <v>64.3416</v>
+      </c>
+      <c r="O8">
+        <v>1.62</v>
+      </c>
+      <c r="P8">
+        <v>3.73</v>
+      </c>
+      <c r="Q8">
+        <v>2694</v>
+      </c>
+      <c r="R8">
+        <v>65955</v>
+      </c>
+      <c r="S8">
+        <v>66315</v>
+      </c>
+      <c r="T8">
+        <v>96.5</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C9">
@@ -668,6 +777,27 @@
       <c r="L9">
         <v>93</v>
       </c>
+      <c r="N9">
+        <v>52.638500000000001</v>
+      </c>
+      <c r="O9">
+        <v>1.61</v>
+      </c>
+      <c r="P9">
+        <v>2.83</v>
+      </c>
+      <c r="Q9">
+        <v>4650</v>
+      </c>
+      <c r="R9">
+        <v>65474</v>
+      </c>
+      <c r="S9">
+        <v>65834</v>
+      </c>
+      <c r="T9">
+        <v>96.4</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C10">
@@ -697,6 +827,27 @@
       <c r="L10">
         <v>95</v>
       </c>
+      <c r="N10">
+        <v>44.31</v>
+      </c>
+      <c r="O10">
+        <v>1.63</v>
+      </c>
+      <c r="P10">
+        <v>3.27</v>
+      </c>
+      <c r="Q10">
+        <v>10353</v>
+      </c>
+      <c r="R10">
+        <v>64993</v>
+      </c>
+      <c r="S10">
+        <v>65353</v>
+      </c>
+      <c r="T10">
+        <v>94.6</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C11">
@@ -726,6 +877,27 @@
       <c r="L11">
         <v>88</v>
       </c>
+      <c r="N11">
+        <v>31.28</v>
+      </c>
+      <c r="O11">
+        <v>1.67</v>
+      </c>
+      <c r="P11">
+        <v>4.2</v>
+      </c>
+      <c r="Q11">
+        <v>8832</v>
+      </c>
+      <c r="R11">
+        <v>64512</v>
+      </c>
+      <c r="S11">
+        <v>64872</v>
+      </c>
+      <c r="T11">
+        <v>94</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C12">
@@ -755,6 +927,27 @@
       <c r="L12">
         <v>77</v>
       </c>
+      <c r="N12">
+        <v>19.646799999999999</v>
+      </c>
+      <c r="O12">
+        <v>1.75</v>
+      </c>
+      <c r="P12">
+        <v>6.5</v>
+      </c>
+      <c r="Q12">
+        <v>8101</v>
+      </c>
+      <c r="R12">
+        <v>64031</v>
+      </c>
+      <c r="S12">
+        <v>64391</v>
+      </c>
+      <c r="T12">
+        <v>92</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C13">
@@ -763,6 +956,27 @@
       <c r="D13">
         <v>4.0653000490000002</v>
       </c>
+      <c r="N13">
+        <v>6.8705999999999996</v>
+      </c>
+      <c r="O13">
+        <v>1.9</v>
+      </c>
+      <c r="P13">
+        <v>6.47</v>
+      </c>
+      <c r="Q13">
+        <v>3683</v>
+      </c>
+      <c r="R13">
+        <v>63478</v>
+      </c>
+      <c r="S13">
+        <v>63838</v>
+      </c>
+      <c r="T13">
+        <v>91</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C14">
@@ -771,6 +985,27 @@
       <c r="D14">
         <v>4.0631000979999996</v>
       </c>
+      <c r="F14">
+        <v>99.847399999999993</v>
+      </c>
+      <c r="G14">
+        <v>1.6</v>
+      </c>
+      <c r="H14">
+        <v>2.4</v>
+      </c>
+      <c r="I14">
+        <v>1965</v>
+      </c>
+      <c r="J14">
+        <v>59169</v>
+      </c>
+      <c r="K14">
+        <v>59529</v>
+      </c>
+      <c r="L14">
+        <v>98</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C15">
@@ -779,6 +1014,27 @@
       <c r="D15">
         <v>4.0609999999999999</v>
       </c>
+      <c r="F15">
+        <v>98.435000000000002</v>
+      </c>
+      <c r="G15">
+        <v>1.57</v>
+      </c>
+      <c r="H15">
+        <v>2.88</v>
+      </c>
+      <c r="I15">
+        <v>5502</v>
+      </c>
+      <c r="J15">
+        <v>59603</v>
+      </c>
+      <c r="K15">
+        <v>59962</v>
+      </c>
+      <c r="L15">
+        <v>96</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C16">
@@ -787,64 +1043,232 @@
       <c r="D16">
         <v>4.0591999510000001</v>
       </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>82.415199999999999</v>
+      </c>
+      <c r="G16">
+        <v>1.55</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>20000</v>
+      </c>
+      <c r="J16">
+        <v>60036</v>
+      </c>
+      <c r="K16">
+        <v>60396</v>
+      </c>
+      <c r="L16">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>99.177726780273971</v>
       </c>
       <c r="D17">
         <v>4.0571000980000003</v>
       </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>71.555099999999996</v>
+      </c>
+      <c r="G17">
+        <v>1.57</v>
+      </c>
+      <c r="H17">
+        <v>2.16</v>
+      </c>
+      <c r="I17">
+        <v>2495</v>
+      </c>
+      <c r="J17">
+        <v>60470</v>
+      </c>
+      <c r="K17">
+        <v>60830</v>
+      </c>
+      <c r="L17">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>99.116845675251142</v>
       </c>
       <c r="D18">
         <v>4.0553999020000004</v>
       </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>61.795400000000001</v>
+      </c>
+      <c r="G18">
+        <v>1.56</v>
+      </c>
+      <c r="H18">
+        <v>2.6</v>
+      </c>
+      <c r="I18">
+        <v>2698</v>
+      </c>
+      <c r="J18">
+        <v>60904</v>
+      </c>
+      <c r="K18">
+        <v>61264</v>
+      </c>
+      <c r="L18">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>99.055964918356167</v>
       </c>
       <c r="D19">
         <v>4.0536000979999995</v>
       </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>50.493200000000002</v>
+      </c>
+      <c r="G19">
+        <v>1.56</v>
+      </c>
+      <c r="H19">
+        <v>3.34</v>
+      </c>
+      <c r="I19">
+        <v>3924</v>
+      </c>
+      <c r="J19">
+        <v>61338</v>
+      </c>
+      <c r="K19">
+        <v>61698</v>
+      </c>
+      <c r="L19">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>98.995083464840178</v>
       </c>
       <c r="D20">
         <v>4.0519999999999996</v>
       </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>37.008000000000003</v>
+      </c>
+      <c r="G20">
+        <v>1.57</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>2313</v>
+      </c>
+      <c r="J20">
+        <v>61772</v>
+      </c>
+      <c r="K20">
+        <v>62132</v>
+      </c>
+      <c r="L20">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>98.934202707945204</v>
       </c>
       <c r="D21">
         <v>4.0503999020000006</v>
       </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>26.348800000000001</v>
+      </c>
+      <c r="G21">
+        <v>1.63</v>
+      </c>
+      <c r="H21">
+        <v>3.39</v>
+      </c>
+      <c r="I21">
+        <v>2381</v>
+      </c>
+      <c r="J21">
+        <v>62206</v>
+      </c>
+      <c r="K21">
+        <v>62566</v>
+      </c>
+      <c r="L21">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>98.873321672694061</v>
       </c>
       <c r="D22">
         <v>4.0488000489999996</v>
       </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>10.1275</v>
+      </c>
+      <c r="G22">
+        <v>1.73</v>
+      </c>
+      <c r="H22">
+        <v>4.87</v>
+      </c>
+      <c r="I22">
+        <v>2559</v>
+      </c>
+      <c r="J22">
+        <v>62640</v>
+      </c>
+      <c r="K22">
+        <v>63000</v>
+      </c>
+      <c r="L22">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>98.812440915799087</v>
       </c>
       <c r="D23">
         <v>4.0476000980000002</v>
       </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1.94</v>
+      </c>
+      <c r="H23">
+        <v>1.37</v>
+      </c>
+      <c r="I23">
+        <v>647</v>
+      </c>
+      <c r="J23">
+        <v>63068</v>
+      </c>
+      <c r="K23">
+        <v>63428</v>
+      </c>
+      <c r="L23">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>98.751559880182654</v>
       </c>
@@ -852,7 +1276,7 @@
         <v>4.0461000980000001</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>98.690679123287666</v>
       </c>
@@ -860,7 +1284,7 @@
         <v>4.044800049</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>98.629797948493149</v>
       </c>
@@ -868,7 +1292,7 @@
         <v>4.0436000979999998</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>98.568916912876716</v>
       </c>
@@ -876,7 +1300,7 @@
         <v>4.0423000489999996</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>98.508035738082185</v>
       </c>
@@ -884,7 +1308,7 @@
         <v>4.0410000000000004</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>98.447154702831057</v>
       </c>
@@ -892,7 +1316,7 @@
         <v>4.0398000490000001</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>98.386273945936068</v>
       </c>
@@ -900,7 +1324,7 @@
         <v>4.0388000489999998</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>98.325392910319636</v>
       </c>
@@ -908,7 +1332,7 @@
         <v>4.0376000979999995</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C32">
         <v>98.264511735525119</v>
       </c>

</xml_diff>